<commit_message>
Added theory 'atom' to all theoretical groups that have also other atoms listed.
</commit_message>
<xml_diff>
--- a/generate/ucan_utoronto_database_production_with_geocode-edited2.xlsx
+++ b/generate/ucan_utoronto_database_production_with_geocode-edited2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="1076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="1081">
   <si>
     <t>name</t>
   </si>
@@ -3250,6 +3250,21 @@
   </si>
   <si>
     <t>South Korea</t>
+  </si>
+  <si>
+    <t>Rb, Er, theory</t>
+  </si>
+  <si>
+    <t>Rb, CsYb, Ca, RbCs, Sr, theory</t>
+  </si>
+  <si>
+    <t>Li, theory</t>
+  </si>
+  <si>
+    <t>He, theory</t>
+  </si>
+  <si>
+    <t>Rb, Li, theory</t>
   </si>
 </sst>
 </file>
@@ -3836,174 +3851,26 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="9">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -4033,75 +3900,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4116,7 +3914,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L241" totalsRowShown="0" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L241" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="A1:L241"/>
   <sortState ref="A2:L248">
     <sortCondition ref="A1:A248"/>
@@ -4130,10 +3928,10 @@
     <tableColumn id="6" name="lat"/>
     <tableColumn id="7" name="long"/>
     <tableColumn id="8" name="exp_theor"/>
-    <tableColumn id="9" name="fields" dataDxfId="38"/>
-    <tableColumn id="10" name="people" dataDxfId="37"/>
-    <tableColumn id="11" name="atom" dataDxfId="36"/>
-    <tableColumn id="12" name="comment" dataDxfId="35"/>
+    <tableColumn id="9" name="fields" dataDxfId="3"/>
+    <tableColumn id="10" name="people" dataDxfId="2"/>
+    <tableColumn id="11" name="atom" dataDxfId="1"/>
+    <tableColumn id="12" name="comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4404,8 +4202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="H201" sqref="H201"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6275,7 +6073,7 @@
         <v>187</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>708</v>
+        <v>1076</v>
       </c>
       <c r="L61" s="5" t="s">
         <v>723</v>
@@ -6782,7 +6580,7 @@
         <v>228</v>
       </c>
       <c r="K78" s="6" t="s">
-        <v>670</v>
+        <v>1077</v>
       </c>
       <c r="L78" s="1" t="s">
         <v>661</v>
@@ -6952,7 +6750,7 @@
         <v>247</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>705</v>
+        <v>1078</v>
       </c>
       <c r="L83" s="1"/>
     </row>
@@ -7608,7 +7406,7 @@
         <v>294</v>
       </c>
       <c r="K105" s="6" t="s">
-        <v>670</v>
+        <v>1077</v>
       </c>
       <c r="L105" s="1" t="s">
         <v>661</v>
@@ -7979,7 +7777,7 @@
         <v>335</v>
       </c>
       <c r="K117" s="6" t="s">
-        <v>673</v>
+        <v>1079</v>
       </c>
       <c r="L117" s="1"/>
     </row>
@@ -8923,7 +8721,7 @@
         <v>416</v>
       </c>
       <c r="K148" s="6" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="L148" s="1" t="s">
         <v>688</v>
@@ -9041,7 +8839,7 @@
         <v>425</v>
       </c>
       <c r="K152" s="6" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="L152" s="1" t="s">
         <v>689</v>
@@ -9073,7 +8871,7 @@
         <v>428</v>
       </c>
       <c r="K153" s="6" t="s">
-        <v>670</v>
+        <v>1077</v>
       </c>
       <c r="L153" s="1" t="s">
         <v>695</v>
@@ -9386,7 +9184,7 @@
         <v>455</v>
       </c>
       <c r="K163" s="6" t="s">
-        <v>670</v>
+        <v>1077</v>
       </c>
       <c r="L163" s="1" t="s">
         <v>695</v>
@@ -9851,7 +9649,7 @@
         <v>501</v>
       </c>
       <c r="K178" s="6" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="L178" s="1" t="s">
         <v>721</v>
@@ -10311,7 +10109,7 @@
         <v>549</v>
       </c>
       <c r="K193" s="6" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="L193" s="1" t="s">
         <v>659</v>
@@ -10405,7 +10203,7 @@
         <v>20</v>
       </c>
       <c r="K196" s="6" t="s">
-        <v>702</v>
+        <v>1080</v>
       </c>
       <c r="L196" s="1"/>
     </row>
@@ -10775,7 +10573,7 @@
         <v>573</v>
       </c>
       <c r="K208" s="6" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="L208" s="1"/>
     </row>
@@ -10958,7 +10756,7 @@
         <v>20</v>
       </c>
       <c r="K214" s="6" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="L214" s="1" t="s">
         <v>674</v>
@@ -11927,7 +11725,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="248" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>844</v>
       </c>
@@ -11959,7 +11757,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="249" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>858</v>
       </c>
@@ -11988,7 +11786,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>867</v>
       </c>
@@ -12017,7 +11815,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="251" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>883</v>
       </c>
@@ -12046,7 +11844,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="252" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>892</v>
       </c>
@@ -12081,7 +11879,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="253" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" ht="270" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>893</v>
       </c>
@@ -12116,7 +11914,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="254" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>903</v>
       </c>
@@ -12142,7 +11940,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="255" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>911</v>
       </c>
@@ -12415,18 +12213,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1:K242">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="4">
       <formula>LEN(TRIM(K1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Exp"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Theory"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Exp/Theory"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Changed last updated file. Uploaded forgotten files.
</commit_message>
<xml_diff>
--- a/generate/ucan_utoronto_database_production_with_geocode-edited2.xlsx
+++ b/generate/ucan_utoronto_database_production_with_geocode-edited2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Work\Ultracool\AllColdAtoms\generate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CF25EA-EB1C-4482-BEF2-A4176370032D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0C9367-309D-48A2-AADF-4968C6100523}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2020" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2020" uniqueCount="1140">
   <si>
     <t>name</t>
   </si>
@@ -3437,9 +3437,6 @@
   </si>
   <si>
     <t>https://www.sussexquantum.com/</t>
-  </si>
-  <si>
-    <t>exp</t>
   </si>
   <si>
     <t>Quantum systems and devices (qsd) group, based at the University of Sussex. We work with Rubdium atoms, and study fundamental questions as well as implementing BEC microscopy.</t>
@@ -4406,7 +4403,7 @@
   <dimension ref="A1:L281"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F131" sqref="F131"/>
+      <selection activeCell="H132" sqref="A1:L257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8402,7 +8399,7 @@
         <v>1137</v>
       </c>
       <c r="C132" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="D132" t="s">
         <v>14</v>
@@ -8414,10 +8411,10 @@
         <v>-8.7287000000000003E-2</v>
       </c>
       <c r="H132" t="s">
+        <v>23</v>
+      </c>
+      <c r="I132" s="8" t="s">
         <v>1138</v>
-      </c>
-      <c r="I132" s="8" t="s">
-        <v>1139</v>
       </c>
       <c r="K132" s="6" t="s">
         <v>654</v>

</xml_diff>